<commit_message>
cleaned unused files and fixed sensitivity on nuclear
</commit_message>
<xml_diff>
--- a/ESM_Italy_13/case_studies/Italy24/scenarios/b.2_NUC_13/inputs/TechProductionMix.xlsx
+++ b/ESM_Italy_13/case_studies/Italy24/scenarios/b.2_NUC_13/inputs/TechProductionMix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tcarm\Documents\GitHub\ESM-Italy\case_studies\Italy24\scenarios\STEPS_NUC\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\ESM-Italy\ESM_Italy_13\case_studies\Italy24\scenarios\b.2_NUC_13\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDBDA95-D801-4F79-96F7-029C8A786CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61C4ACF-2057-4FDD-93FE-CBED7E161811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1452" yWindow="156" windowWidth="17676" windowHeight="12084" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="r.A" sheetId="1" r:id="rId1"/>
@@ -545,19 +545,19 @@
       <pane xSplit="1" ySplit="2" topLeftCell="I27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O43" sqref="O43"/>
+      <selection pane="bottomRight" activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="14" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +649,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
@@ -741,7 +741,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1990</v>
       </c>
@@ -764,7 +764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1991</v>
       </c>
@@ -787,7 +787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1992</v>
       </c>
@@ -810,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1993</v>
       </c>
@@ -833,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1994</v>
       </c>
@@ -856,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1995</v>
       </c>
@@ -879,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1996</v>
       </c>
@@ -902,7 +902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1997</v>
       </c>
@@ -925,7 +925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1998</v>
       </c>
@@ -948,7 +948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>1999</v>
       </c>
@@ -971,7 +971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2000</v>
       </c>
@@ -994,7 +994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2001</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2002</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2003</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2004</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2005</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2006</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2007</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2008</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2009</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2010</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2011</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2012</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2013</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2014</v>
       </c>
@@ -1277,7 +1277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2015</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2016</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2017</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2018</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2019</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2020</v>
       </c>
@@ -1379,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2021</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2022</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2023</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2024</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2025</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2026</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2027</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2028</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2029</v>
       </c>
@@ -1511,31 +1511,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2030</v>
       </c>
       <c r="K43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="O43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2031</v>
       </c>
       <c r="K44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="O44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2032</v>
       </c>
       <c r="K45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="O45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2033</v>
       </c>
@@ -1543,7 +1552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2034</v>
       </c>
@@ -1551,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2035</v>
       </c>
@@ -1559,7 +1568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2036</v>
       </c>
@@ -1567,7 +1576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2037</v>
       </c>
@@ -1575,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>2038</v>
       </c>
@@ -1583,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>2039</v>
       </c>
@@ -1591,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>2040</v>
       </c>
@@ -1599,7 +1608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>2041</v>
       </c>
@@ -1607,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>2042</v>
       </c>
@@ -1615,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>2043</v>
       </c>
@@ -1623,7 +1632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>2044</v>
       </c>
@@ -1631,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>2045</v>
       </c>
@@ -1639,7 +1648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>2046</v>
       </c>
@@ -1647,7 +1656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>2047</v>
       </c>
@@ -1655,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>2048</v>
       </c>
@@ -1663,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>2049</v>
       </c>
@@ -1671,7 +1680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>2050</v>
       </c>
@@ -1679,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>2051</v>
       </c>
@@ -1687,7 +1696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>2052</v>
       </c>
@@ -1695,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>2053</v>
       </c>
@@ -1703,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>2054</v>
       </c>
@@ -1711,7 +1720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>2055</v>
       </c>
@@ -1719,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2056</v>
       </c>
@@ -1727,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>2057</v>
       </c>
@@ -1735,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>2058</v>
       </c>
@@ -1743,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>2059</v>
       </c>
@@ -1751,7 +1760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>2060</v>
       </c>
@@ -1759,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>2061</v>
       </c>
@@ -1767,7 +1776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>2062</v>
       </c>
@@ -1775,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>2063</v>
       </c>
@@ -1783,7 +1792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>2064</v>
       </c>
@@ -1791,7 +1800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>2065</v>
       </c>
@@ -1799,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>2066</v>
       </c>
@@ -1807,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>2067</v>
       </c>
@@ -1815,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>2068</v>
       </c>
@@ -1823,7 +1832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>2069</v>
       </c>
@@ -1831,7 +1840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>2070</v>
       </c>

</xml_diff>